<commit_message>
Another change to Phone list
</commit_message>
<xml_diff>
--- a/PhoneCell.xlsx
+++ b/PhoneCell.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Steph Lackerdas</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -261,7 +261,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>dfakadf</t>
+    <t>Mason</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>443-6600</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -699,8 +703,11 @@
       <c r="B7">
         <v>8183899331</v>
       </c>
+      <c r="D7" t="s">
+        <v>60</v>
+      </c>
       <c r="E7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1134,6 +1141,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>